<commit_message>
add new data integration
</commit_message>
<xml_diff>
--- a/codes/feature_groups.xlsx
+++ b/codes/feature_groups.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\d\Projects\!Projects\PG_portal\script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\d\Projects\!Projects\PG_portal\script\codes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0658A0-FE9D-4034-9837-9E9E3A26D703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD65295E-4756-471C-A439-55EE0ACD4F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5563" uniqueCount="2191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5563" uniqueCount="2195">
   <si>
     <t>Category Name</t>
   </si>
@@ -6611,6 +6611,18 @@
   </si>
   <si>
     <t>product_lvls</t>
+  </si>
+  <si>
+    <t>Synergetic Super Concentrated Kids &amp; Sensitive</t>
+  </si>
+  <si>
+    <t>Synergetic Super Concentrated Universal</t>
+  </si>
+  <si>
+    <t>Klassicheskoye Not Applicable Universal</t>
+  </si>
+  <si>
+    <t>Vestar brand Super Concentrated Universal</t>
   </si>
 </sst>
 </file>
@@ -6696,7 +6708,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6980,7 +6994,7 @@
   <dimension ref="A1:J1108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6992,7 +7006,7 @@
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="10.54296875" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" customWidth="1"/>
+    <col min="8" max="8" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -7023,7 +7037,7 @@
       <c r="I1" t="s">
         <v>1094</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" t="s">
         <v>2190</v>
       </c>
     </row>
@@ -39489,8 +39503,8 @@
       <c r="G985">
         <v>6127</v>
       </c>
-      <c r="H985" t="s">
-        <v>1049</v>
+      <c r="H985" s="7" t="s">
+        <v>2194</v>
       </c>
       <c r="I985" t="s">
         <v>2065</v>
@@ -39885,8 +39899,8 @@
       <c r="G997">
         <v>6139</v>
       </c>
-      <c r="H997" t="s">
-        <v>951</v>
+      <c r="H997" s="7" t="s">
+        <v>2193</v>
       </c>
       <c r="I997" t="s">
         <v>2077</v>
@@ -41634,7 +41648,7 @@
       <c r="G1050">
         <v>6192</v>
       </c>
-      <c r="H1050" t="s">
+      <c r="H1050" s="9" t="s">
         <v>862</v>
       </c>
       <c r="I1050" t="s">
@@ -41667,8 +41681,8 @@
       <c r="G1051">
         <v>6193</v>
       </c>
-      <c r="H1051" t="s">
-        <v>862</v>
+      <c r="H1051" s="9" t="s">
+        <v>2191</v>
       </c>
       <c r="I1051" t="s">
         <v>2130</v>
@@ -41700,8 +41714,8 @@
       <c r="G1052">
         <v>6194</v>
       </c>
-      <c r="H1052" t="s">
-        <v>862</v>
+      <c r="H1052" s="9" t="s">
+        <v>2192</v>
       </c>
       <c r="I1052" t="s">
         <v>2131</v>

</xml_diff>